<commit_message>
added time for twitter sentiment analysis
</commit_message>
<xml_diff>
--- a/Docs/Work.xlsx
+++ b/Docs/Work.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Anmol Shukla</t>
   </si>
@@ -81,6 +81,15 @@
   </si>
   <si>
     <t>75% PPT completed</t>
+  </si>
+  <si>
+    <t>4th Mar</t>
+  </si>
+  <si>
+    <t>60 min</t>
+  </si>
+  <si>
+    <t>Twitter sentiment analysis</t>
   </si>
 </sst>
 </file>
@@ -132,14 +141,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -448,16 +457,16 @@
   <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="5"/>
       <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
@@ -470,7 +479,9 @@
       <c r="F1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="2"/>
+      <c r="G1" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -489,10 +500,10 @@
       <c r="W1" s="1"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="4"/>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
@@ -524,10 +535,10 @@
       <c r="W2" s="1"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
@@ -559,10 +570,10 @@
       <c r="W3" s="1"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
@@ -594,10 +605,10 @@
       <c r="W4" s="1"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
@@ -610,7 +621,9 @@
       <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -629,24 +642,26 @@
       <c r="W5" s="1"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="G6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="3"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -662,47 +677,52 @@
       <c r="U6" s="2"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="F6:F10"/>
+    <mergeCell ref="G6:G10"/>
     <mergeCell ref="H6:H10"/>
     <mergeCell ref="A6:B10"/>
     <mergeCell ref="A4:B4"/>
@@ -710,11 +730,6 @@
     <mergeCell ref="C6:C10"/>
     <mergeCell ref="D6:D10"/>
     <mergeCell ref="E6:E10"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="F6:F10"/>
-    <mergeCell ref="G6:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>